<commit_message>
all cases run for integration testing now
Still need to add hvac elements and address sunspace to finish measure.
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="51200" windowHeight="28260" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2305,7 +2305,7 @@
     <t>standard_reports.eui</t>
   </si>
   <si>
-    <t>BESTEST 0620-02b (no_weather ideal air lhs)</t>
+    <t>BESTEST 0624_01b</t>
   </si>
 </sst>
 </file>
@@ -4137,10 +4137,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1559">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6284,7 +6284,7 @@
       <c r="D23" s="26"/>
       <c r="E23" s="22"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" ht="28">
       <c r="A24" s="22" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-2))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-2))</f>
         <v>Number of Samples</v>
@@ -6603,7 +6603,7 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="4">
+  <dataValidations disablePrompts="1" count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
       <formula1>AnalysisType</formula1>
     </dataValidation>
@@ -6688,14 +6688,14 @@
       <c r="R1" s="30"/>
       <c r="S1" s="27"/>
       <c r="T1" s="27"/>
-      <c r="U1" s="44" t="s">
+      <c r="U1" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15">
       <c r="A2" s="31" t="s">
@@ -6885,7 +6885,7 @@
         <v>747</v>
       </c>
       <c r="O5" s="42"/>
-      <c r="P5" s="45" t="s">
+      <c r="P5" s="44" t="s">
         <v>750</v>
       </c>
       <c r="Q5" s="42"/>

</xml_diff>

<commit_message>
Adding zone ventilation design flow rate
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="562"/>
@@ -2305,7 +2305,7 @@
     <t>standard_reports.eui</t>
   </si>
   <si>
-    <t>BESTEST 0624_01d (setback)</t>
+    <t>BESTEST 0627_02 (finished night vent)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added Custom Logic or Sunspace case
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="51200" windowHeight="28260" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="51200" windowHeight="28260" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2305,7 +2305,7 @@
     <t>standard_reports.eui</t>
   </si>
   <si>
-    <t>BESTEST 0628_01 (surf prop)</t>
+    <t>BESTEST 0628_02 (sun space)</t>
   </si>
 </sst>
 </file>
@@ -2483,8 +2483,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1559">
+  <cellStyleXfs count="1565">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4142,7 +4148,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1559">
+  <cellStyles count="1565">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4922,6 +4928,9 @@
     <cellStyle name="Followed Hyperlink" xfId="1554" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1556" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1564" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5701,6 +5710,9 @@
     <cellStyle name="Hyperlink" xfId="1553" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1555" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1563" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6002,7 +6014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -6632,7 +6644,7 @@
   <dimension ref="A1:Z53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8262,11 +8274,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M92"/>
+  <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8452,29 +8464,31 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="1:13" s="22" customFormat="1">
+    <row r="6" spans="1:13">
       <c r="A6" s="15" t="s">
-        <v>650</v>
-      </c>
-      <c r="B6" s="15"/>
+        <v>751</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>752</v>
+      </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>689</v>
+        <v>753</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>651</v>
+        <v>738</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>63</v>
       </c>
       <c r="G6" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="15" t="b">
         <v>1</v>
       </c>
       <c r="I6" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
@@ -8483,12 +8497,12 @@
     </row>
     <row r="7" spans="1:13" s="22" customFormat="1">
       <c r="A7" s="15" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>651</v>
@@ -8512,12 +8526,12 @@
     </row>
     <row r="8" spans="1:13" s="22" customFormat="1">
       <c r="A8" s="15" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>651</v>
@@ -8541,15 +8555,15 @@
     </row>
     <row r="9" spans="1:13" s="22" customFormat="1">
       <c r="A9" s="15" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>63</v>
@@ -8570,15 +8584,15 @@
     </row>
     <row r="10" spans="1:13" s="22" customFormat="1">
       <c r="A10" s="15" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>657</v>
+        <v>692</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>467</v>
+        <v>655</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>63</v>
@@ -8599,12 +8613,12 @@
     </row>
     <row r="11" spans="1:13" s="22" customFormat="1">
       <c r="A11" s="15" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>467</v>
@@ -8628,12 +8642,12 @@
     </row>
     <row r="12" spans="1:13" s="22" customFormat="1">
       <c r="A12" s="15" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>467</v>
@@ -8657,12 +8671,12 @@
     </row>
     <row r="13" spans="1:13" s="22" customFormat="1">
       <c r="A13" s="15" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>467</v>
@@ -8686,12 +8700,12 @@
     </row>
     <row r="14" spans="1:13" s="22" customFormat="1">
       <c r="A14" s="15" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>467</v>
@@ -8713,14 +8727,14 @@
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
     </row>
-    <row r="15" spans="1:13" s="21" customFormat="1">
+    <row r="15" spans="1:13" s="22" customFormat="1">
       <c r="A15" s="15" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>467</v>
@@ -8744,12 +8758,12 @@
     </row>
     <row r="16" spans="1:13" s="21" customFormat="1">
       <c r="A16" s="15" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>467</v>
@@ -8773,12 +8787,12 @@
     </row>
     <row r="17" spans="1:13" s="21" customFormat="1">
       <c r="A17" s="15" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>467</v>
@@ -8802,12 +8816,12 @@
     </row>
     <row r="18" spans="1:13" s="21" customFormat="1">
       <c r="A18" s="15" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>467</v>
@@ -8831,12 +8845,12 @@
     </row>
     <row r="19" spans="1:13" s="21" customFormat="1">
       <c r="A19" s="15" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>467</v>
@@ -8860,12 +8874,12 @@
     </row>
     <row r="20" spans="1:13" s="21" customFormat="1">
       <c r="A20" s="15" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>467</v>
@@ -8887,14 +8901,14 @@
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
     </row>
-    <row r="21" spans="1:13" s="22" customFormat="1">
+    <row r="21" spans="1:13" s="21" customFormat="1">
       <c r="A21" s="15" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>467</v>
@@ -8918,12 +8932,12 @@
     </row>
     <row r="22" spans="1:13" s="22" customFormat="1">
       <c r="A22" s="15" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>467</v>
@@ -8947,12 +8961,12 @@
     </row>
     <row r="23" spans="1:13" s="22" customFormat="1">
       <c r="A23" s="15" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>467</v>
@@ -8976,15 +8990,15 @@
     </row>
     <row r="24" spans="1:13" s="22" customFormat="1">
       <c r="A24" s="15" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>686</v>
+        <v>467</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>63</v>
@@ -9003,31 +9017,29 @@
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" s="22" customFormat="1">
       <c r="A25" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>752</v>
-      </c>
+        <v>684</v>
+      </c>
+      <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15" t="s">
-        <v>753</v>
+        <v>685</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>738</v>
+        <v>686</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>63</v>
       </c>
       <c r="G25" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" s="15" t="b">
         <v>1</v>
       </c>
       <c r="I25" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
@@ -9035,19 +9047,7 @@
       <c r="M25" s="15"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
+      <c r="B26" s="21"/>
     </row>
     <row r="27" spans="1:13">
       <c r="B27" s="21"/>
@@ -9243,9 +9243,6 @@
     </row>
     <row r="91" spans="2:2">
       <c r="B91" s="21"/>
-    </row>
-    <row r="92" spans="2:2">
-      <c r="B92" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
weather file working on server
Not able to get it to assign weather file on apply measures now.
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -2283,9 +2283,6 @@
     <t>Case Number</t>
   </si>
   <si>
-    <t>../weather/DRYCOLDTMY.epw</t>
-  </si>
-  <si>
     <t>EUI</t>
   </si>
   <si>
@@ -2304,7 +2301,10 @@
     <t>|600 - Base Case|</t>
   </si>
   <si>
-    <t>BESTEST 0629_02 (Output Variablesl)</t>
+    <t>../weather/USA_MA_Boston-Logan.Intl.AP.725090_TMY3.epw</t>
+  </si>
+  <si>
+    <t>BESTEST 0630_1 (Weather)</t>
   </si>
 </sst>
 </file>
@@ -4051,7 +4051,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4103,9 +4103,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -6296,7 +6293,7 @@
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,1,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,1,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v>individual_variables / all_variables</v>
       </c>
-      <c r="D23" s="26"/>
+      <c r="D23" s="25"/>
       <c r="E23" s="22"/>
     </row>
     <row r="24" spans="1:6" ht="28">
@@ -6311,7 +6308,7 @@
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="25">
         <v>40</v>
       </c>
       <c r="E24" s="22"/>
@@ -6329,7 +6326,7 @@
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,3,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,3,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v/>
       </c>
-      <c r="D25" s="26"/>
+      <c r="D25" s="25"/>
       <c r="E25" s="22"/>
     </row>
     <row r="26" spans="1:6" s="22" customFormat="1">
@@ -6345,7 +6342,7 @@
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,4,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,4,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v/>
       </c>
-      <c r="D26" s="26"/>
+      <c r="D26" s="25"/>
     </row>
     <row r="27" spans="1:6" s="22" customFormat="1">
       <c r="A27" s="22" t="str">
@@ -6360,7 +6357,7 @@
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,5,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,5,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v/>
       </c>
-      <c r="D27" s="26"/>
+      <c r="D27" s="25"/>
     </row>
     <row r="28" spans="1:6" s="22" customFormat="1">
       <c r="A28" s="22" t="str">
@@ -6375,7 +6372,7 @@
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,6,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,6,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v/>
       </c>
-      <c r="D28" s="26"/>
+      <c r="D28" s="25"/>
     </row>
     <row r="29" spans="1:6" s="22" customFormat="1">
       <c r="A29" s="22" t="str">
@@ -6390,7 +6387,7 @@
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,7,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,7,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v/>
       </c>
-      <c r="D29" s="26"/>
+      <c r="D29" s="25"/>
     </row>
     <row r="30" spans="1:6" s="22" customFormat="1">
       <c r="A30" s="22" t="str">
@@ -6405,7 +6402,7 @@
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,8,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,8,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v/>
       </c>
-      <c r="D30" s="26"/>
+      <c r="D30" s="25"/>
     </row>
     <row r="31" spans="1:6" s="22" customFormat="1">
       <c r="A31" s="22" t="str">
@@ -6420,7 +6417,7 @@
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,9,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,9,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v/>
       </c>
-      <c r="D31" s="26"/>
+      <c r="D31" s="25"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="22" t="str">
@@ -6435,7 +6432,7 @@
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,10,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,10,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v/>
       </c>
-      <c r="D32" s="26"/>
+      <c r="D32" s="25"/>
       <c r="E32" s="22"/>
     </row>
     <row r="33" spans="1:6" s="22" customFormat="1">
@@ -6451,7 +6448,7 @@
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$32,11,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$32,11,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v/>
       </c>
-      <c r="D33" s="26"/>
+      <c r="D33" s="25"/>
     </row>
     <row r="34" spans="1:6" s="22" customFormat="1">
       <c r="A34" s="22" t="str">
@@ -6519,15 +6516,15 @@
       <c r="A38" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="25" t="s">
-        <v>747</v>
+      <c r="B38" s="16" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" ht="28">
       <c r="A40" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="39" t="s">
+      <c r="B40" s="38" t="s">
         <v>454</v>
       </c>
       <c r="C40" s="6" t="s">
@@ -6677,244 +6674,244 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="29" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="28" t="s">
         <v>472</v>
       </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="30" t="s">
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29" t="s">
         <v>473</v>
       </c>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="45" t="s">
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="30" t="s">
         <v>546</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="30" t="s">
         <v>545</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
     </row>
     <row r="3" spans="1:26" s="9" customFormat="1" ht="45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="32" t="s">
         <v>632</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="L3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="35" t="s">
+      <c r="M3" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="35" t="s">
+      <c r="N3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="35" t="s">
+      <c r="O3" s="34" t="s">
         <v>544</v>
       </c>
-      <c r="P3" s="35" t="s">
+      <c r="P3" s="34" t="s">
         <v>474</v>
       </c>
-      <c r="Q3" s="35" t="s">
+      <c r="Q3" s="34" t="s">
         <v>475</v>
       </c>
-      <c r="R3" s="32" t="s">
+      <c r="R3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="S3" s="32" t="s">
+      <c r="S3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="T3" s="32" t="s">
+      <c r="T3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="U3" s="32" t="s">
+      <c r="U3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="32" t="s">
+      <c r="V3" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="W3" s="32" t="s">
+      <c r="W3" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="X3" s="32" t="s">
+      <c r="X3" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="Y3" s="32" t="s">
+      <c r="Y3" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="Z3" s="32"/>
-    </row>
-    <row r="4" spans="1:26" s="40" customFormat="1" ht="15">
-      <c r="A4" s="37" t="b">
+      <c r="Z3" s="31"/>
+    </row>
+    <row r="4" spans="1:26" s="39" customFormat="1" ht="15">
+      <c r="A4" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>742</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="36" t="s">
         <v>743</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="36" t="s">
         <v>744</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-      <c r="X4" s="37"/>
-      <c r="Y4" s="37"/>
-      <c r="Z4" s="37"/>
-    </row>
-    <row r="5" spans="1:26" s="43" customFormat="1" ht="15">
-      <c r="A5" s="38"/>
-      <c r="B5" s="38" t="s">
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="36"/>
+    </row>
+    <row r="5" spans="1:26" s="42" customFormat="1" ht="15">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="37" t="s">
         <v>746</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="37" t="s">
         <v>745</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38" t="s">
+      <c r="F5" s="37"/>
+      <c r="G5" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38" t="s">
+      <c r="H5" s="37"/>
+      <c r="I5" s="37" t="s">
+        <v>751</v>
+      </c>
+      <c r="J5" s="37" t="s">
         <v>752</v>
       </c>
-      <c r="J5" s="38" t="s">
-        <v>753</v>
-      </c>
-      <c r="K5" s="38" t="s">
-        <v>752</v>
-      </c>
-      <c r="L5" s="38" t="s">
-        <v>752</v>
-      </c>
-      <c r="M5" s="38" t="s">
-        <v>752</v>
-      </c>
-      <c r="N5" s="38" t="s">
-        <v>752</v>
-      </c>
-      <c r="O5" s="42"/>
-      <c r="P5" s="44" t="s">
+      <c r="K5" s="37" t="s">
         <v>751</v>
       </c>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="38" t="s">
+      <c r="L5" s="37" t="s">
+        <v>751</v>
+      </c>
+      <c r="M5" s="37" t="s">
+        <v>751</v>
+      </c>
+      <c r="N5" s="37" t="s">
+        <v>751</v>
+      </c>
+      <c r="O5" s="41"/>
+      <c r="P5" s="43" t="s">
+        <v>750</v>
+      </c>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="37" t="s">
         <v>737</v>
       </c>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
-      <c r="W5" s="38"/>
-      <c r="X5" s="38"/>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
+      <c r="Z5" s="37"/>
     </row>
     <row r="6" spans="1:26" customFormat="1" ht="15">
       <c r="A6" s="10"/>
@@ -7097,11 +7094,11 @@
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
       <c r="R12" s="15"/>
       <c r="S12" s="15"/>
       <c r="T12" s="15"/>
@@ -7181,11 +7178,11 @@
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
       <c r="R15" s="15"/>
       <c r="S15" s="15"/>
       <c r="T15" s="15"/>
@@ -7265,11 +7262,11 @@
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="36"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
       <c r="R18" s="15"/>
       <c r="S18" s="15"/>
       <c r="T18" s="15"/>
@@ -7349,11 +7346,11 @@
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
       <c r="R21" s="15"/>
       <c r="S21" s="15"/>
       <c r="T21" s="15"/>
@@ -7433,11 +7430,11 @@
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="36"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="35"/>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -7547,8 +7544,8 @@
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
-      <c r="O28" s="36"/>
-      <c r="P28" s="36"/>
+      <c r="O28" s="35"/>
+      <c r="P28" s="35"/>
       <c r="Q28" s="15"/>
       <c r="R28" s="15"/>
       <c r="S28" s="15"/>
@@ -7715,8 +7712,8 @@
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
       <c r="N34" s="10"/>
-      <c r="O34" s="36"/>
-      <c r="P34" s="36"/>
+      <c r="O34" s="35"/>
+      <c r="P34" s="35"/>
       <c r="Q34" s="15"/>
       <c r="R34" s="15"/>
       <c r="S34" s="15"/>
@@ -7911,8 +7908,8 @@
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
       <c r="N41" s="15"/>
-      <c r="O41" s="36"/>
-      <c r="P41" s="36"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="35"/>
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
       <c r="S41" s="15"/>
@@ -7967,8 +7964,8 @@
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
       <c r="N43" s="15"/>
-      <c r="O43" s="36"/>
-      <c r="P43" s="36"/>
+      <c r="O43" s="35"/>
+      <c r="P43" s="35"/>
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
       <c r="S43" s="15"/>
@@ -7995,8 +7992,8 @@
       <c r="L44" s="15"/>
       <c r="M44" s="15"/>
       <c r="N44" s="15"/>
-      <c r="O44" s="36"/>
-      <c r="P44" s="36"/>
+      <c r="O44" s="35"/>
+      <c r="P44" s="35"/>
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
       <c r="S44" s="15"/>
@@ -8051,8 +8048,8 @@
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
-      <c r="O46" s="36"/>
-      <c r="P46" s="36"/>
+      <c r="O46" s="35"/>
+      <c r="P46" s="35"/>
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
       <c r="S46" s="15"/>
@@ -8107,8 +8104,8 @@
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
       <c r="N48" s="15"/>
-      <c r="O48" s="36"/>
-      <c r="P48" s="36"/>
+      <c r="O48" s="35"/>
+      <c r="P48" s="35"/>
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
       <c r="S48" s="15"/>
@@ -8163,8 +8160,8 @@
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
       <c r="N50" s="15"/>
-      <c r="O50" s="36"/>
-      <c r="P50" s="36"/>
+      <c r="O50" s="35"/>
+      <c r="P50" s="35"/>
       <c r="Q50" s="15"/>
       <c r="R50" s="15"/>
       <c r="S50" s="15"/>
@@ -8219,8 +8216,8 @@
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
       <c r="N52" s="15"/>
-      <c r="O52" s="36"/>
-      <c r="P52" s="36"/>
+      <c r="O52" s="35"/>
+      <c r="P52" s="35"/>
       <c r="Q52" s="15"/>
       <c r="R52" s="15"/>
       <c r="S52" s="15"/>
@@ -8303,97 +8300,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="22" customFormat="1" ht="18">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27" t="s">
         <v>466</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" ht="15">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>460</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>633</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="31" t="s">
         <v>613</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="31" t="s">
         <v>461</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="31" t="s">
         <v>614</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="31" t="s">
         <v>615</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="31" t="s">
         <v>616</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="31" t="s">
         <v>617</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="31" t="s">
         <v>618</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="M2" s="32"/>
+      <c r="M2" s="31"/>
     </row>
     <row r="3" spans="1:13" s="9" customFormat="1" ht="45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>620</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>634</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>621</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>622</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="31" t="s">
         <v>623</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="31" t="s">
         <v>462</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="31" t="s">
         <v>462</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="31" t="s">
         <v>462</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="J3" s="33" t="s">
         <v>624</v>
       </c>
-      <c r="K3" s="32" t="s">
+      <c r="K3" s="31" t="s">
         <v>624</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="31" t="s">
         <v>625</v>
       </c>
-      <c r="M3" s="32"/>
+      <c r="M3" s="31"/>
     </row>
     <row r="4" spans="1:13" s="22" customFormat="1">
       <c r="A4" s="15" t="s">
@@ -8469,14 +8466,14 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>748</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>749</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>738</v>

</xml_diff>

<commit_message>
adding measure to spreadsheet
odd things happening in server and GUI with multiple reporting measures.
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2195" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="758">
   <si>
     <t>type</t>
   </si>
@@ -2304,7 +2304,16 @@
     <t>../weather/USA_MA_Boston-Logan.Intl.AP.725090_TMY3.epw</t>
   </si>
   <si>
-    <t>BESTEST 0630_1 (Weather)</t>
+    <t>BESTEST Building Thermal Envelope and Fabric Load Reports</t>
+  </si>
+  <si>
+    <t>BESTESTBuildingThermalEnvelopeAndFabricLoadReports</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports</t>
+  </si>
+  <si>
+    <t>BESTEST 06705_01 (reporting measure)</t>
   </si>
 </sst>
 </file>
@@ -2482,8 +2491,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1567">
+  <cellStyleXfs count="1569">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4146,7 +4157,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1567">
+  <cellStyles count="1569">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4930,6 +4941,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1562" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1564" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1568" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5713,6 +5725,7 @@
     <cellStyle name="Hyperlink" xfId="1561" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1563" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1567" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6186,7 +6199,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>470</v>
@@ -6644,7 +6657,7 @@
   <dimension ref="A1:Z53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6913,33 +6926,43 @@
       <c r="Y5" s="37"/>
       <c r="Z5" s="37"/>
     </row>
-    <row r="6" spans="1:26" customFormat="1" ht="15">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
+    <row r="6" spans="1:26" s="39" customFormat="1" ht="15">
+      <c r="A6" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>754</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>756</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>755</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="36"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="36"/>
+      <c r="X6" s="36"/>
+      <c r="Y6" s="36"/>
+      <c r="Z6" s="36"/>
     </row>
     <row r="7" spans="1:26" customFormat="1" ht="15">
       <c r="A7" s="10"/>

</xml_diff>

<commit_message>
updating reporting module name
It was getting stepped on by methods in standard report. Unless the
module is really the same it should have unique name.
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28260" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2313,7 +2313,7 @@
     <t>bestest_building_thermal_envelope_and_fabric_load_reports</t>
   </si>
   <si>
-    <t>BESTEST 06705_01 (reporting measure)</t>
+    <t>BESTEST 06706_01c (updated module name)</t>
   </si>
 </sst>
 </file>
@@ -6656,8 +6656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
initial cvs output from server
I need to add more register values to this.
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28260" tabRatio="562"/>
+    <workbookView xWindow="25600" yWindow="-20" windowWidth="25600" windowHeight="28260" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="747">
   <si>
     <t>type</t>
   </si>
@@ -2010,99 +2010,6 @@
     <t>m2</t>
   </si>
   <si>
-    <t>Natural Gas Heating Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.heating_natural_gas</t>
-  </si>
-  <si>
-    <t>Cooling Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.cooling_electricity</t>
-  </si>
-  <si>
-    <t>Interior Lighting Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_lighting_electricity</t>
-  </si>
-  <si>
-    <t>Exterior Lighting Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.exterior_lighting_electricity</t>
-  </si>
-  <si>
-    <t>Equipment Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_equipment_electricity</t>
-  </si>
-  <si>
-    <t>Equipment Natural Gas Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_equipment_natural_gas</t>
-  </si>
-  <si>
-    <t>Experior Equipment Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.exterior_equipment_electricity</t>
-  </si>
-  <si>
-    <t>Fans Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.fans_electricity</t>
-  </si>
-  <si>
-    <t>Pumps Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.pumps_electricity</t>
-  </si>
-  <si>
-    <t>Heat Rejection Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.heat_rejection_electricity</t>
-  </si>
-  <si>
-    <t>Humidification Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.humidification_electricity</t>
-  </si>
-  <si>
-    <t>Water Systems Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.water_systems_electricity</t>
-  </si>
-  <si>
-    <t>Water Systems Natural Gas Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.water_systems_natural_gas</t>
-  </si>
-  <si>
-    <t>Refrigeration Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.refrigeration_electricity</t>
-  </si>
-  <si>
-    <t>Total Life Cycle Cost</t>
-  </si>
-  <si>
-    <t>standard_report.total_life_cycle_cost</t>
-  </si>
-  <si>
-    <t>$</t>
-  </si>
-  <si>
     <t>NG EUI</t>
   </si>
   <si>
@@ -2313,7 +2220,67 @@
     <t>bestest_building_thermal_envelope_and_fabric_load_reports</t>
   </si>
   <si>
-    <t>BESTEST 06712a (1.12.1 run)</t>
+    <t>Annual Cooling</t>
+  </si>
+  <si>
+    <t>MWh</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.annual_cooling</t>
+  </si>
+  <si>
+    <t>Ann Clg (MWh)</t>
+  </si>
+  <si>
+    <t>Annual Heating</t>
+  </si>
+  <si>
+    <t>Ann Htg (MWh)</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.annual_heating</t>
+  </si>
+  <si>
+    <t>Peak Heating Value</t>
+  </si>
+  <si>
+    <t>Peak Cooling Value</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>Peak Htg Time</t>
+  </si>
+  <si>
+    <t>Peak Clg Time</t>
+  </si>
+  <si>
+    <t>Peak Htg Value</t>
+  </si>
+  <si>
+    <t>Peak Clg Value</t>
+  </si>
+  <si>
+    <t>Peak Heating Time</t>
+  </si>
+  <si>
+    <t>Peak Cooling Time</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.peak_heating_value</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.peak_cooling_value</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.peak_cooling_time_display_name</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.peak_heating_time_display_name</t>
+  </si>
+  <si>
+    <t>BESTEST 06712d (adjsting peak time output)</t>
   </si>
 </sst>
 </file>
@@ -2491,7 +2458,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1569">
+  <cellStyleXfs count="1587">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4061,8 +4028,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4156,8 +4141,9 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1569">
+  <cellStyles count="1587">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4942,6 +4928,15 @@
     <cellStyle name="Followed Hyperlink" xfId="1564" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1566" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1586" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5726,6 +5721,15 @@
     <cellStyle name="Hyperlink" xfId="1563" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1565" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1585" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6066,7 +6070,7 @@
         <v>435</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>706</v>
+        <v>675</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>436</v>
@@ -6077,7 +6081,7 @@
         <v>457</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>722</v>
+        <v>691</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>458</v>
@@ -6088,7 +6092,7 @@
         <v>468</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>739</v>
+        <v>708</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>609</v>
@@ -6099,7 +6103,7 @@
         <v>469</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>723</v>
+        <v>692</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>471</v>
@@ -6167,21 +6171,21 @@
         <v>$1.96/hour</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>705</v>
+        <v>674</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="22" customFormat="1" ht="28">
       <c r="A10" s="22" t="s">
-        <v>695</v>
+        <v>664</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>696</v>
+        <v>665</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="2" t="s">
-        <v>697</v>
+        <v>666</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="7" customFormat="1">
@@ -6199,7 +6203,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>757</v>
+        <v>746</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>470</v>
@@ -6210,7 +6214,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>740</v>
+        <v>709</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -6530,7 +6534,7 @@
         <v>28</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>753</v>
+        <v>722</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" ht="28">
@@ -6556,13 +6560,13 @@
         <v>31</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>736</v>
+        <v>705</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>40</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>741</v>
+        <v>710</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>449</v>
@@ -6586,18 +6590,18 @@
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1" ht="56">
       <c r="A46" s="6" t="s">
-        <v>698</v>
+        <v>667</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>699</v>
+        <v>668</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>700</v>
+        <v>669</v>
       </c>
       <c r="D46" s="18"/>
       <c r="E46" s="18"/>
       <c r="F46" s="8" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="2" customFormat="1">
@@ -6612,18 +6616,18 @@
     </row>
     <row r="49" spans="1:6" s="2" customFormat="1" ht="42">
       <c r="A49" s="6" t="s">
-        <v>702</v>
+        <v>671</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>703</v>
+        <v>672</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>700</v>
+        <v>669</v>
       </c>
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
       <c r="F49" s="8" t="s">
-        <v>704</v>
+        <v>673</v>
       </c>
     </row>
   </sheetData>
@@ -6841,13 +6845,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>742</v>
+        <v>711</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>743</v>
+        <v>712</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>744</v>
+        <v>713</v>
       </c>
       <c r="E4" s="36" t="s">
         <v>67</v>
@@ -6881,10 +6885,10 @@
       </c>
       <c r="C5" s="37"/>
       <c r="D5" s="37" t="s">
-        <v>746</v>
+        <v>715</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>745</v>
+        <v>714</v>
       </c>
       <c r="F5" s="37"/>
       <c r="G5" s="37" t="s">
@@ -6892,30 +6896,30 @@
       </c>
       <c r="H5" s="37"/>
       <c r="I5" s="37" t="s">
-        <v>751</v>
+        <v>720</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>752</v>
+        <v>721</v>
       </c>
       <c r="K5" s="37" t="s">
-        <v>751</v>
+        <v>720</v>
       </c>
       <c r="L5" s="37" t="s">
-        <v>751</v>
+        <v>720</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>751</v>
+        <v>720</v>
       </c>
       <c r="N5" s="37" t="s">
-        <v>751</v>
+        <v>720</v>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="43" t="s">
-        <v>750</v>
+        <v>719</v>
       </c>
       <c r="Q5" s="41"/>
       <c r="R5" s="37" t="s">
-        <v>737</v>
+        <v>706</v>
       </c>
       <c r="S5" s="37"/>
       <c r="T5" s="37"/>
@@ -6931,13 +6935,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>754</v>
+        <v>723</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>756</v>
+        <v>725</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>755</v>
+        <v>724</v>
       </c>
       <c r="E6" s="36" t="s">
         <v>232</v>
@@ -8297,19 +8301,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M91"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="54.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
@@ -8339,7 +8343,7 @@
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="15">
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="30">
       <c r="A2" s="31" t="s">
         <v>460</v>
       </c>
@@ -8378,7 +8382,7 @@
       </c>
       <c r="M2" s="31"/>
     </row>
-    <row r="3" spans="1:13" s="9" customFormat="1" ht="45">
+    <row r="3" spans="1:13" s="9" customFormat="1" ht="60">
       <c r="A3" s="31" t="s">
         <v>620</v>
       </c>
@@ -8420,7 +8424,7 @@
         <v>626</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>687</v>
+        <v>656</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>627</v>
@@ -8455,7 +8459,7 @@
         <v>629</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>688</v>
+        <v>657</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>630</v>
@@ -8489,17 +8493,17 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="15" t="s">
-        <v>747</v>
+        <v>716</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>748</v>
+        <v>717</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>749</v>
+        <v>718</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>738</v>
+        <v>707</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>63</v>
@@ -8525,7 +8529,7 @@
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>689</v>
+        <v>658</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>651</v>
@@ -8537,7 +8541,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="15" t="b">
         <v>0</v>
@@ -8554,7 +8558,7 @@
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>690</v>
+        <v>659</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>651</v>
@@ -8566,7 +8570,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="15" t="b">
         <v>0</v>
@@ -8583,7 +8587,7 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>691</v>
+        <v>660</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>651</v>
@@ -8595,7 +8599,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="15" t="b">
         <v>0</v>
@@ -8612,7 +8616,7 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>692</v>
+        <v>661</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>655</v>
@@ -8624,7 +8628,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="15" t="b">
         <v>0</v>
@@ -8634,460 +8638,207 @@
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
     </row>
-    <row r="11" spans="1:13" s="22" customFormat="1">
-      <c r="A11" s="15" t="s">
-        <v>656</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15" t="s">
-        <v>657</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="F11" s="15" t="s">
+    <row r="11" spans="1:13">
+      <c r="A11" s="45" t="s">
+        <v>730</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>731</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>732</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>727</v>
+      </c>
+      <c r="F11" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="15" t="b">
+      <c r="G11" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="I11" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-    </row>
-    <row r="12" spans="1:13" s="22" customFormat="1">
-      <c r="A12" s="15" t="s">
-        <v>658</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15" t="s">
-        <v>659</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="F12" s="15" t="s">
+      <c r="H11" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="45" t="s">
+        <v>726</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>729</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="45" t="s">
+        <v>728</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>727</v>
+      </c>
+      <c r="F12" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="15" t="b">
+      <c r="G12" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="I12" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-    </row>
-    <row r="13" spans="1:13" s="22" customFormat="1">
-      <c r="A13" s="15" t="s">
-        <v>660</v>
-      </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15" t="s">
-        <v>661</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="F13" s="15" t="s">
+      <c r="H12" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="45" t="s">
+        <v>733</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>738</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="45" t="s">
+        <v>742</v>
+      </c>
+      <c r="E13" s="45" t="s">
+        <v>735</v>
+      </c>
+      <c r="F13" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="15" t="b">
+      <c r="G13" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="I13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-    </row>
-    <row r="14" spans="1:13" s="22" customFormat="1">
-      <c r="A14" s="15" t="s">
-        <v>662</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15" t="s">
-        <v>663</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="F14" s="15" t="s">
+      <c r="H13" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="45" t="s">
+        <v>734</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>739</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="45" t="s">
+        <v>743</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>735</v>
+      </c>
+      <c r="F14" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="15" t="b">
+      <c r="G14" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="I14" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
+      <c r="H14" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="45" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:13" s="22" customFormat="1">
-      <c r="A15" s="15" t="s">
-        <v>664</v>
-      </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
-        <v>665</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="15" t="b">
+      <c r="A15" s="45" t="s">
+        <v>740</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>736</v>
+      </c>
+      <c r="D15" s="45" t="s">
+        <v>745</v>
+      </c>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="I15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-    </row>
-    <row r="16" spans="1:13" s="21" customFormat="1">
-      <c r="A16" s="15" t="s">
-        <v>666</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15" t="s">
-        <v>667</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="15" t="b">
+      <c r="H15" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="I16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-    </row>
-    <row r="17" spans="1:13" s="21" customFormat="1">
-      <c r="A17" s="15" t="s">
-        <v>668</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15" t="s">
-        <v>669</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="15" t="b">
+      <c r="I15" s="45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="22" customFormat="1">
+      <c r="A16" s="45" t="s">
+        <v>741</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>737</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>744</v>
+      </c>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="I17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-    </row>
-    <row r="18" spans="1:13" s="21" customFormat="1">
-      <c r="A18" s="15" t="s">
-        <v>670</v>
-      </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15" t="s">
-        <v>671</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="15" t="b">
+      <c r="H16" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="I18" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-    </row>
-    <row r="19" spans="1:13" s="21" customFormat="1">
-      <c r="A19" s="15" t="s">
-        <v>672</v>
-      </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15" t="s">
-        <v>673</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-    </row>
-    <row r="20" spans="1:13" s="21" customFormat="1">
-      <c r="A20" s="15" t="s">
-        <v>674</v>
-      </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15" t="s">
-        <v>675</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-    </row>
-    <row r="21" spans="1:13" s="21" customFormat="1">
-      <c r="A21" s="15" t="s">
-        <v>676</v>
-      </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15" t="s">
-        <v>677</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-    </row>
-    <row r="22" spans="1:13" s="22" customFormat="1">
-      <c r="A22" s="15" t="s">
-        <v>678</v>
-      </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15" t="s">
-        <v>679</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-    </row>
-    <row r="23" spans="1:13" s="22" customFormat="1">
-      <c r="A23" s="15" t="s">
-        <v>680</v>
-      </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15" t="s">
-        <v>681</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-    </row>
-    <row r="24" spans="1:13" s="22" customFormat="1">
-      <c r="A24" s="15" t="s">
-        <v>682</v>
-      </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15" t="s">
-        <v>683</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G24" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I24" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-    </row>
-    <row r="25" spans="1:13" s="22" customFormat="1">
-      <c r="A25" s="15" t="s">
-        <v>684</v>
-      </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15" t="s">
-        <v>685</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>686</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="I16" s="45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="21"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="21"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="21"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="21"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="21"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="21"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="21"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="21"/>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="21"/>
+    </row>
+    <row r="26" spans="2:2">
       <c r="B26" s="21"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="2:2">
       <c r="B27" s="21"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="2:2">
       <c r="B28" s="21"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="2:2">
       <c r="B29" s="21"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="2:2">
       <c r="B30" s="21"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="2:2">
       <c r="B31" s="21"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="2:2">
       <c r="B32" s="21"/>
     </row>
     <row r="33" spans="2:2">
@@ -9221,51 +8972,6 @@
     </row>
     <row r="76" spans="2:2">
       <c r="B76" s="21"/>
-    </row>
-    <row r="77" spans="2:2">
-      <c r="B77" s="21"/>
-    </row>
-    <row r="78" spans="2:2">
-      <c r="B78" s="21"/>
-    </row>
-    <row r="79" spans="2:2">
-      <c r="B79" s="21"/>
-    </row>
-    <row r="80" spans="2:2">
-      <c r="B80" s="21"/>
-    </row>
-    <row r="81" spans="2:2">
-      <c r="B81" s="21"/>
-    </row>
-    <row r="82" spans="2:2">
-      <c r="B82" s="21"/>
-    </row>
-    <row r="83" spans="2:2">
-      <c r="B83" s="21"/>
-    </row>
-    <row r="84" spans="2:2">
-      <c r="B84" s="21"/>
-    </row>
-    <row r="85" spans="2:2">
-      <c r="B85" s="21"/>
-    </row>
-    <row r="86" spans="2:2">
-      <c r="B86" s="21"/>
-    </row>
-    <row r="87" spans="2:2">
-      <c r="B87" s="21"/>
-    </row>
-    <row r="88" spans="2:2">
-      <c r="B88" s="21"/>
-    </row>
-    <row r="89" spans="2:2">
-      <c r="B89" s="21"/>
-    </row>
-    <row r="90" spans="2:2">
-      <c r="B90" s="21"/>
-    </row>
-    <row r="91" spans="2:2">
-      <c r="B91" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -17565,7 +17271,7 @@
         <v>642</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>693</v>
+        <v>662</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="21" customFormat="1">
@@ -17582,7 +17288,7 @@
         <v>640</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>693</v>
+        <v>662</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="21" customFormat="1">
@@ -17599,7 +17305,7 @@
         <v>641</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>694</v>
+        <v>663</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="21" customFormat="1">
@@ -17616,7 +17322,7 @@
         <v>643</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>694</v>
+        <v>663</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -17633,7 +17339,7 @@
         <v>645</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>694</v>
+        <v>663</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="21" customFormat="1"/>
@@ -17686,7 +17392,7 @@
         <v>548</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>729</v>
+        <v>698</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
@@ -17706,18 +17412,18 @@
         <v>551</v>
       </c>
       <c r="X18" s="21" t="s">
-        <v>712</v>
+        <v>681</v>
       </c>
       <c r="Y18" s="21"/>
       <c r="Z18" s="21"/>
       <c r="AA18" t="s">
-        <v>707</v>
+        <v>676</v>
       </c>
       <c r="AD18" t="s">
-        <v>708</v>
+        <v>677</v>
       </c>
       <c r="AG18" s="21" t="s">
-        <v>724</v>
+        <v>693</v>
       </c>
       <c r="AH18" s="21"/>
       <c r="AI18" s="21"/>
@@ -17727,13 +17433,13 @@
         <v>548</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>730</v>
+        <v>699</v>
       </c>
       <c r="G19" s="21">
         <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>735</v>
+        <v>704</v>
       </c>
       <c r="I19" t="s">
         <v>569</v>
@@ -17772,16 +17478,16 @@
         <v>578</v>
       </c>
       <c r="X19" s="21" t="s">
-        <v>721</v>
+        <v>690</v>
       </c>
       <c r="Y19" s="21" t="s">
-        <v>714</v>
+        <v>683</v>
       </c>
       <c r="Z19" s="21" t="s">
-        <v>714</v>
+        <v>683</v>
       </c>
       <c r="AD19" s="21" t="s">
-        <v>709</v>
+        <v>678</v>
       </c>
       <c r="AE19" s="21">
         <v>30</v>
@@ -17790,27 +17496,27 @@
         <v>587</v>
       </c>
       <c r="AG19" s="21" t="s">
-        <v>725</v>
+        <v>694</v>
       </c>
       <c r="AH19" s="21" t="b">
         <v>1</v>
       </c>
       <c r="AI19" s="21" t="s">
-        <v>726</v>
+        <v>695</v>
       </c>
     </row>
     <row r="20" spans="1:35">
       <c r="A20" s="21" t="s">
-        <v>729</v>
+        <v>698</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>731</v>
+        <v>700</v>
       </c>
       <c r="G20" s="21">
         <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>734</v>
+        <v>703</v>
       </c>
       <c r="I20" t="s">
         <v>4</v>
@@ -17855,16 +17561,16 @@
         <v>2</v>
       </c>
       <c r="Z20" s="21" t="s">
-        <v>713</v>
+        <v>682</v>
       </c>
       <c r="AG20" s="21" t="s">
-        <v>727</v>
+        <v>696</v>
       </c>
       <c r="AH20" s="21" t="b">
         <v>1</v>
       </c>
       <c r="AI20" s="21" t="s">
-        <v>728</v>
+        <v>697</v>
       </c>
     </row>
     <row r="21" spans="1:35">
@@ -17872,7 +17578,7 @@
         <v>15</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>732</v>
+        <v>701</v>
       </c>
       <c r="G21" s="21">
         <v>1</v>
@@ -17914,10 +17620,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>733</v>
+        <v>702</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>733</v>
+        <v>702</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>557</v>
@@ -17961,13 +17667,13 @@
         <v>539</v>
       </c>
       <c r="O23" s="21" t="s">
-        <v>717</v>
+        <v>686</v>
       </c>
       <c r="P23" s="21">
         <v>1</v>
       </c>
       <c r="Q23" s="22" t="s">
-        <v>718</v>
+        <v>687</v>
       </c>
       <c r="R23" s="22" t="s">
         <v>566</v>
@@ -18022,13 +17728,13 @@
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
       <c r="L25" s="21" t="s">
-        <v>710</v>
+        <v>679</v>
       </c>
       <c r="M25" s="22">
         <v>0</v>
       </c>
       <c r="N25" s="22" t="s">
-        <v>711</v>
+        <v>680</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>537</v>
@@ -18040,18 +17746,18 @@
         <v>576</v>
       </c>
       <c r="R25" s="22" t="s">
-        <v>719</v>
+        <v>688</v>
       </c>
       <c r="S25" s="21">
         <v>2</v>
       </c>
       <c r="T25" s="21" t="s">
-        <v>720</v>
+        <v>689</v>
       </c>
     </row>
     <row r="26" spans="1:35">
       <c r="A26" t="s">
-        <v>712</v>
+        <v>681</v>
       </c>
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
@@ -18074,7 +17780,7 @@
     </row>
     <row r="27" spans="1:35">
       <c r="A27" t="s">
-        <v>707</v>
+        <v>676</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -18100,7 +17806,7 @@
     </row>
     <row r="28" spans="1:35">
       <c r="A28" t="s">
-        <v>708</v>
+        <v>677</v>
       </c>
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
@@ -18115,18 +17821,18 @@
         <v>573</v>
       </c>
       <c r="R28" t="s">
-        <v>710</v>
+        <v>679</v>
       </c>
       <c r="S28" s="22">
         <v>0</v>
       </c>
       <c r="T28" s="22" t="s">
-        <v>711</v>
+        <v>680</v>
       </c>
     </row>
     <row r="29" spans="1:35">
       <c r="A29" s="21" t="s">
-        <v>724</v>
+        <v>693</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
@@ -18157,13 +17863,13 @@
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
       <c r="O31" s="21" t="s">
-        <v>710</v>
+        <v>679</v>
       </c>
       <c r="P31" s="22">
         <v>0</v>
       </c>
       <c r="Q31" s="22" t="s">
-        <v>711</v>
+        <v>680</v>
       </c>
     </row>
     <row r="32" spans="1:35">
@@ -18171,13 +17877,13 @@
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
       <c r="O32" t="s">
-        <v>715</v>
+        <v>684</v>
       </c>
       <c r="P32" s="22">
         <v>1</v>
       </c>
       <c r="Q32" s="22" t="s">
-        <v>716</v>
+        <v>685</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated registerValues and results CSV
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-20" windowWidth="25600" windowHeight="28260" tabRatio="562"/>
+    <workbookView xWindow="25600" yWindow="-20" windowWidth="25600" windowHeight="28260" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="769">
   <si>
     <t>type</t>
   </si>
@@ -2280,7 +2280,73 @@
     <t>bestest_building_thermal_envelope_and_fabric_load_reports.peak_heating_time_display_name</t>
   </si>
   <si>
-    <t>BESTEST 06712d (adjsting peak time output)</t>
+    <t>BESTEST 06715a (csv_update)</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.sens_htg_clg_0104</t>
+  </si>
+  <si>
+    <t>Annual Heating and Cooling</t>
+  </si>
+  <si>
+    <t>Ann Htg and Clg</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.temp_0104</t>
+  </si>
+  <si>
+    <t>Temperature January 4th</t>
+  </si>
+  <si>
+    <t>Temp 0104</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.temp_0727</t>
+  </si>
+  <si>
+    <t>Temp 0727</t>
+  </si>
+  <si>
+    <t>Temperature July 27th</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.surf_out_inst_slr_rad_0305_zone_surface_south</t>
+  </si>
+  <si>
+    <t>Surface Incident South March 5th</t>
+  </si>
+  <si>
+    <t>Surface Incident West March 5th</t>
+  </si>
+  <si>
+    <t>Incident South 0305</t>
+  </si>
+  <si>
+    <t>Incident West 0305</t>
+  </si>
+  <si>
+    <t>Surface Incident South July 22nd</t>
+  </si>
+  <si>
+    <t>Surface Incident West July 22nd</t>
+  </si>
+  <si>
+    <t>Incident South 0722</t>
+  </si>
+  <si>
+    <t>Incident West 0722</t>
+  </si>
+  <si>
+    <t>1 deg C Temperature Bins</t>
+  </si>
+  <si>
+    <t>Temp Bins</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.temp_bins</t>
   </si>
 </sst>
 </file>
@@ -2458,8 +2524,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1587">
+  <cellStyleXfs count="1625">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4138,12 +4242,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1587">
+  <cellStyles count="1625">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4937,6 +5041,25 @@
     <cellStyle name="Followed Hyperlink" xfId="1582" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1584" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1612" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1624" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5730,6 +5853,25 @@
     <cellStyle name="Hyperlink" xfId="1581" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1583" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1607" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1609" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1611" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1613" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1617" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1619" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1621" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1623" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6031,7 +6173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -6717,14 +6859,14 @@
       <c r="R1" s="29"/>
       <c r="S1" s="26"/>
       <c r="T1" s="26"/>
-      <c r="U1" s="44" t="s">
+      <c r="U1" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15">
       <c r="A2" s="30" t="s">
@@ -8303,9 +8445,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8639,206 +8781,376 @@
       <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>730</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>731</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="44" t="s">
         <v>732</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="44" t="s">
         <v>727</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="F11" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="45" t="b">
+      <c r="G11" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="H11" s="45" t="b">
+      <c r="H11" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="I11" s="45" t="b">
+      <c r="I11" s="44" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="44" t="s">
         <v>726</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>729</v>
       </c>
       <c r="C12" s="22"/>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="44" t="s">
         <v>728</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="44" t="s">
         <v>727</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F12" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="45" t="b">
+      <c r="G12" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="H12" s="45" t="b">
+      <c r="H12" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="I12" s="45" t="b">
+      <c r="I12" s="44" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="44" t="s">
         <v>733</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>738</v>
       </c>
       <c r="C13" s="22"/>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="44" t="s">
         <v>742</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="44" t="s">
         <v>735</v>
       </c>
-      <c r="F13" s="45" t="s">
+      <c r="F13" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="45" t="b">
+      <c r="G13" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="H13" s="45" t="b">
+      <c r="H13" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="I13" s="45" t="b">
+      <c r="I13" s="44" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="44" t="s">
         <v>734</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>739</v>
       </c>
       <c r="C14" s="22"/>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="44" t="s">
         <v>743</v>
       </c>
-      <c r="E14" s="45" t="s">
+      <c r="E14" s="44" t="s">
         <v>735</v>
       </c>
-      <c r="F14" s="45" t="s">
+      <c r="F14" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="45" t="b">
+      <c r="G14" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="H14" s="45" t="b">
+      <c r="H14" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="I14" s="45" t="b">
+      <c r="I14" s="44" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="22" customFormat="1">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="44" t="s">
         <v>740</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>736</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D15" s="44" t="s">
         <v>745</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45" t="s">
+      <c r="E15" s="44"/>
+      <c r="F15" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="G15" s="45" t="b">
+      <c r="G15" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="45" t="b">
+      <c r="H15" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="I15" s="45" t="b">
+      <c r="I15" s="44" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="22" customFormat="1">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="44" t="s">
         <v>741</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>737</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="44" t="s">
         <v>744</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45" t="s">
+      <c r="E16" s="44"/>
+      <c r="F16" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="G16" s="45" t="b">
+      <c r="G16" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="H16" s="45" t="b">
+      <c r="H16" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="I16" s="45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="21"/>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="21"/>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="21"/>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="21"/>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="21"/>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="21"/>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="21"/>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="21"/>
-    </row>
-    <row r="25" spans="2:2">
+      <c r="I16" s="44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="44" t="s">
+        <v>748</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>749</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>747</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="44" t="s">
+        <v>751</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>752</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>750</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="F18" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="44" t="s">
+        <v>756</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>755</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>754</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>753</v>
+      </c>
+      <c r="F19" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="44" t="s">
+        <v>758</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>760</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>757</v>
+      </c>
+      <c r="F20" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="44" t="s">
+        <v>759</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>761</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>757</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="44" t="s">
+        <v>762</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>764</v>
+      </c>
+      <c r="D22" s="44" t="s">
+        <v>757</v>
+      </c>
+      <c r="F22" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="44" t="s">
+        <v>763</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>765</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>757</v>
+      </c>
+      <c r="F23" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="44" t="s">
+        <v>766</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>767</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>768</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="B25" s="21"/>
-    </row>
-    <row r="26" spans="2:2">
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+    </row>
+    <row r="26" spans="1:9">
       <c r="B26" s="21"/>
     </row>
-    <row r="27" spans="2:2">
+    <row r="27" spans="1:9">
       <c r="B27" s="21"/>
     </row>
-    <row r="28" spans="2:2">
+    <row r="28" spans="1:9">
       <c r="B28" s="21"/>
     </row>
-    <row r="29" spans="2:2">
+    <row r="29" spans="1:9">
       <c r="B29" s="21"/>
     </row>
-    <row r="30" spans="2:2">
+    <row r="30" spans="1:9">
       <c r="B30" s="21"/>
     </row>
-    <row r="31" spans="2:2">
+    <row r="31" spans="1:9">
       <c r="B31" s="21"/>
     </row>
-    <row r="32" spans="2:2">
+    <row r="32" spans="1:9">
       <c r="B32" s="21"/>
     </row>
     <row r="33" spans="2:2">

</xml_diff>

<commit_message>
updated min,max,avg, and hourly ff temps
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-20" windowWidth="25600" windowHeight="28260" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="25600" yWindow="-20" windowWidth="25600" windowHeight="28260" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="778">
   <si>
     <t>type</t>
   </si>
@@ -2280,9 +2280,6 @@
     <t>bestest_building_thermal_envelope_and_fabric_load_reports.peak_heating_time_display_name</t>
   </si>
   <si>
-    <t>BESTEST 06715a (csv_update)</t>
-  </si>
-  <si>
     <t>bestest_building_thermal_envelope_and_fabric_load_reports.sens_htg_clg_0104</t>
   </si>
   <si>
@@ -2328,18 +2325,6 @@
     <t>Incident West 0305</t>
   </si>
   <si>
-    <t>Surface Incident South July 22nd</t>
-  </si>
-  <si>
-    <t>Surface Incident West July 22nd</t>
-  </si>
-  <si>
-    <t>Incident South 0722</t>
-  </si>
-  <si>
-    <t>Incident West 0722</t>
-  </si>
-  <si>
     <t>1 deg C Temperature Bins</t>
   </si>
   <si>
@@ -2347,6 +2332,48 @@
   </si>
   <si>
     <t>bestest_building_thermal_envelope_and_fabric_load_reports.temp_bins</t>
+  </si>
+  <si>
+    <t>Min Temp</t>
+  </si>
+  <si>
+    <t>Max Temp</t>
+  </si>
+  <si>
+    <t>Avg Temp</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.max_temp</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.min_temp</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.avg_temp</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.surf_out_inst_slr_rad_0305_zone_surface_west</t>
+  </si>
+  <si>
+    <t>Surface Incident South July 27th</t>
+  </si>
+  <si>
+    <t>Surface Incident West July 27th</t>
+  </si>
+  <si>
+    <t>Incident South 0727</t>
+  </si>
+  <si>
+    <t>Incident West 0727</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.surf_out_inst_slr_rad_0727_zone_surface_west</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.surf_out_inst_slr_rad_0727_zone_surface_south</t>
+  </si>
+  <si>
+    <t>BESTEST 06718e (min temp fix)</t>
   </si>
 </sst>
 </file>
@@ -2524,8 +2551,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1625">
+  <cellStyleXfs count="1629">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4247,7 +4278,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1625">
+  <cellStyles count="1629">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5060,6 +5091,8 @@
     <cellStyle name="Followed Hyperlink" xfId="1620" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1622" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1626" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1628" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5872,6 +5905,8 @@
     <cellStyle name="Hyperlink" xfId="1619" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1621" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1623" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1625" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1627" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6173,7 +6208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -6345,7 +6380,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>746</v>
+        <v>777</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>470</v>
@@ -8445,14 +8480,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="54.83203125" style="1" customWidth="1"/>
@@ -8937,13 +8972,13 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="44" t="s">
+        <v>747</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>748</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>749</v>
-      </c>
       <c r="D17" s="44" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F17" s="44" t="s">
         <v>103</v>
@@ -8960,16 +8995,16 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="44" t="s">
+        <v>750</v>
+      </c>
+      <c r="B18" s="21" t="s">
         <v>751</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="D18" s="44" t="s">
+        <v>749</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>752</v>
-      </c>
-      <c r="D18" s="44" t="s">
-        <v>750</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>753</v>
       </c>
       <c r="F18" s="44" t="s">
         <v>63</v>
@@ -8986,16 +9021,16 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="44" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D19" s="44" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="F19" s="44" t="s">
         <v>63</v>
@@ -9012,13 +9047,13 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="44" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="F20" s="44" t="s">
         <v>103</v>
@@ -9035,13 +9070,13 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="44" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D21" s="44" t="s">
-        <v>757</v>
+        <v>770</v>
       </c>
       <c r="F21" s="44" t="s">
         <v>103</v>
@@ -9058,13 +9093,13 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="44" t="s">
-        <v>762</v>
+        <v>771</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>764</v>
+        <v>773</v>
       </c>
       <c r="D22" s="44" t="s">
-        <v>757</v>
+        <v>776</v>
       </c>
       <c r="F22" s="44" t="s">
         <v>103</v>
@@ -9081,13 +9116,13 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="44" t="s">
-        <v>763</v>
+        <v>772</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>765</v>
+        <v>774</v>
       </c>
       <c r="D23" s="44" t="s">
-        <v>757</v>
+        <v>775</v>
       </c>
       <c r="F23" s="44" t="s">
         <v>103</v>
@@ -9104,13 +9139,13 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="44" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="D24" s="44" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="F24" s="44" t="s">
         <v>103</v>
@@ -9126,17 +9161,77 @@
       </c>
     </row>
     <row r="25" spans="1:9">
+      <c r="A25" s="44" t="s">
+        <v>764</v>
+      </c>
       <c r="B25" s="21"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="44" t="s">
+        <v>767</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>752</v>
+      </c>
+      <c r="F25" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="44" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:9">
+      <c r="A26" s="44" t="s">
+        <v>765</v>
+      </c>
       <c r="B26" s="21"/>
+      <c r="D26" s="44" t="s">
+        <v>768</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>752</v>
+      </c>
+      <c r="F26" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="44" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:9">
+      <c r="A27" s="44" t="s">
+        <v>766</v>
+      </c>
       <c r="B27" s="21"/>
+      <c r="D27" s="44" t="s">
+        <v>769</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>752</v>
+      </c>
+      <c r="F27" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="44" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:9">
       <c r="B28" s="21"/>

</xml_diff>

<commit_message>
Sunspace fix for boundary condition, ideal air, and thermostats
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-20" windowWidth="25600" windowHeight="28260" tabRatio="562"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2373,7 +2373,7 @@
     <t>bestest_building_thermal_envelope_and_fabric_load_reports.surf_out_inst_slr_rad_0727_zone_surface_south</t>
   </si>
   <si>
-    <t>BESTEST 06718f - htg clg fix</t>
+    <t>BESTEST 060805 (SunSpace Fix)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
misc measure bug fixes in 5-2A (envelope)
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="21060" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2373,7 +2373,7 @@
     <t>bestest_building_thermal_envelope_and_fabric_load_reports.surf_out_inst_slr_rad_0727_zone_surface_south</t>
   </si>
   <si>
-    <t>BESTEST 060805 (SunSpace Fix)</t>
+    <t>BESTEST 06080e (night vent)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Populated solar incident and transmission
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="21060" tabRatio="562"/>
+    <workbookView xWindow="25600" yWindow="-20" windowWidth="25600" windowHeight="28260" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2237" uniqueCount="791">
   <si>
     <t>type</t>
   </si>
@@ -2373,7 +2373,46 @@
     <t>bestest_building_thermal_envelope_and_fabric_load_reports.surf_out_inst_slr_rad_0727_zone_surface_south</t>
   </si>
   <si>
-    <t>BESTEST 06080e (night vent)</t>
+    <t>North Incident Solar</t>
+  </si>
+  <si>
+    <t>East Incident Solar</t>
+  </si>
+  <si>
+    <t>West Incident Solar</t>
+  </si>
+  <si>
+    <t>South Incident Solar</t>
+  </si>
+  <si>
+    <t>Horizontal Incident Solar</t>
+  </si>
+  <si>
+    <t>Zone Total Transmitted Beam Solar</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.zone_total_transmitted_beam_solar_radiation</t>
+  </si>
+  <si>
+    <t>kWh/m^2</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.north_incident_solar_radiation</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.east_incident_solar_radiation</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.west_incident_solar_radiation</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.horizontal_incident_solar_radiation</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.south_incident_solar_radiation</t>
+  </si>
+  <si>
+    <t>BESTEST 0908 (added south incident)</t>
   </si>
 </sst>
 </file>
@@ -2551,8 +2590,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1629">
+  <cellStyleXfs count="1639">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4278,7 +4327,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1629">
+  <cellStyles count="1639">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5093,6 +5142,11 @@
     <cellStyle name="Followed Hyperlink" xfId="1624" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1626" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1628" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1630" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1632" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1634" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1636" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1638" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5907,6 +5961,11 @@
     <cellStyle name="Hyperlink" xfId="1623" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1625" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1627" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1629" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1631" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1633" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1635" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1637" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6380,7 +6439,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>777</v>
+        <v>790</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>470</v>
@@ -8482,7 +8541,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9234,66 +9293,198 @@
       </c>
     </row>
     <row r="28" spans="1:9">
+      <c r="A28" s="44" t="s">
+        <v>777</v>
+      </c>
       <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="44" t="s">
+        <v>785</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="F28" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="44" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:9">
+      <c r="A29" s="44" t="s">
+        <v>778</v>
+      </c>
       <c r="B29" s="21"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="44" t="s">
+        <v>786</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="44" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:9">
+      <c r="A30" s="44" t="s">
+        <v>779</v>
+      </c>
       <c r="B30" s="21"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="44" t="s">
+        <v>787</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="F30" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="44" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:9">
+      <c r="A31" s="44" t="s">
+        <v>780</v>
+      </c>
       <c r="B31" s="21"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="44" t="s">
+        <v>789</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="F31" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="44" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:9">
+      <c r="A32" s="44" t="s">
+        <v>781</v>
+      </c>
       <c r="B32" s="21"/>
-    </row>
-    <row r="33" spans="2:2">
+      <c r="C32" s="22"/>
+      <c r="D32" s="44" t="s">
+        <v>788</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="F32" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="44" t="s">
+        <v>782</v>
+      </c>
       <c r="B33" s="21"/>
-    </row>
-    <row r="34" spans="2:2">
+      <c r="C33" s="22"/>
+      <c r="D33" s="44" t="s">
+        <v>783</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="F33" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="B34" s="21"/>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="1:9">
       <c r="B35" s="21"/>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="1:9">
       <c r="B36" s="21"/>
     </row>
-    <row r="37" spans="2:2">
+    <row r="37" spans="1:9">
       <c r="B37" s="21"/>
     </row>
-    <row r="38" spans="2:2">
+    <row r="38" spans="1:9">
       <c r="B38" s="21"/>
     </row>
-    <row r="39" spans="2:2">
+    <row r="39" spans="1:9">
       <c r="B39" s="21"/>
     </row>
-    <row r="40" spans="2:2">
+    <row r="40" spans="1:9">
       <c r="B40" s="21"/>
     </row>
-    <row r="41" spans="2:2">
+    <row r="41" spans="1:9">
       <c r="B41" s="21"/>
     </row>
-    <row r="42" spans="2:2">
+    <row r="42" spans="1:9">
       <c r="B42" s="21"/>
     </row>
-    <row r="43" spans="2:2">
+    <row r="43" spans="1:9">
       <c r="B43" s="21"/>
     </row>
-    <row r="44" spans="2:2">
+    <row r="44" spans="1:9">
       <c r="B44" s="21"/>
     </row>
-    <row r="45" spans="2:2">
+    <row r="45" spans="1:9">
       <c r="B45" s="21"/>
     </row>
-    <row r="46" spans="2:2">
+    <row r="46" spans="1:9">
       <c r="B46" s="21"/>
     </row>
-    <row r="47" spans="2:2">
+    <row r="47" spans="1:9">
       <c r="B47" s="21"/>
     </row>
-    <row r="48" spans="2:2">
+    <row r="48" spans="1:9">
       <c r="B48" s="21"/>
     </row>
     <row r="49" spans="2:2">

</xml_diff>

<commit_message>
added time stamp to min and max temp
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-20" windowWidth="25600" windowHeight="28260" tabRatio="562"/>
+    <workbookView xWindow="25600" yWindow="-20" windowWidth="25600" windowHeight="28260" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2237" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2243" uniqueCount="795">
   <si>
     <t>type</t>
   </si>
@@ -2412,7 +2412,19 @@
     <t>bestest_building_thermal_envelope_and_fabric_load_reports.south_incident_solar_radiation</t>
   </si>
   <si>
-    <t>BESTEST 0908 (added south incident)</t>
+    <t>Max Temp Position</t>
+  </si>
+  <si>
+    <t>Min Temp Position</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.max_index_position</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.min_index_position</t>
+  </si>
+  <si>
+    <t>BESTEST 0908c (added min max temp index position)</t>
   </si>
 </sst>
 </file>
@@ -2590,8 +2602,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1639">
+  <cellStyleXfs count="1659">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4327,7 +4359,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1639">
+  <cellStyles count="1659">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5147,6 +5179,16 @@
     <cellStyle name="Followed Hyperlink" xfId="1634" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1636" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1638" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1640" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1642" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1658" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5966,6 +6008,16 @@
     <cellStyle name="Hyperlink" xfId="1633" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1635" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1637" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1639" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1641" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1643" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1645" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1657" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6267,7 +6319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -6439,7 +6491,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>470</v>
@@ -8539,9 +8591,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9221,7 +9273,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="44" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
@@ -9246,7 +9298,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="44" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B26" s="21"/>
       <c r="D26" s="44" t="s">
@@ -9442,11 +9494,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" s="22" customFormat="1">
+      <c r="A34" s="44" t="s">
+        <v>790</v>
+      </c>
       <c r="B34" s="21"/>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="D34" s="44" t="s">
+        <v>792</v>
+      </c>
+      <c r="F34" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="22" customFormat="1">
+      <c r="A35" s="44" t="s">
+        <v>791</v>
+      </c>
       <c r="B35" s="21"/>
+      <c r="D35" s="44" t="s">
+        <v>793</v>
+      </c>
+      <c r="F35" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="44" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:9">
       <c r="B36" s="21"/>

</xml_diff>

<commit_message>
fix to tilmestep and ideal air loads in 2a
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-20" windowWidth="25600" windowHeight="28260" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="23460" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2424,7 +2424,7 @@
     <t>bestest_building_thermal_envelope_and_fabric_load_reports.min_index_position</t>
   </si>
   <si>
-    <t>BESTEST 0908c (added min max temp index position)</t>
+    <t>BESTEST 1024_b (ideal air and sim timestep)</t>
   </si>
 </sst>
 </file>
@@ -6319,7 +6319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -8591,7 +8591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>

</xml_diff>

<commit_message>
fixes issue #13 case 395 geometry
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -2388,12 +2388,6 @@
     <t>Horizontal Incident Solar</t>
   </si>
   <si>
-    <t>Zone Total Transmitted Beam Solar</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.zone_total_transmitted_beam_solar_radiation</t>
-  </si>
-  <si>
     <t>kWh/m^2</t>
   </si>
   <si>
@@ -2424,7 +2418,13 @@
     <t>bestest_building_thermal_envelope_and_fabric_load_reports.min_index_position</t>
   </si>
   <si>
-    <t>BESTEST 1024_e2 (updating var to bestest_os_server_output)</t>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reports.zone_total_transmitted_solar_radiation</t>
+  </si>
+  <si>
+    <t>Zone Total Transmitted Solar</t>
+  </si>
+  <si>
+    <t>BESTEST 1024_g (fixing output in spreadsheet for beam radiation)</t>
   </si>
 </sst>
 </file>
@@ -8593,7 +8593,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8601,7 +8601,7 @@
     <col min="1" max="1" width="33.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="54.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="104.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
@@ -9351,10 +9351,10 @@
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
       <c r="D28" s="44" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F28" s="44" t="s">
         <v>63</v>
@@ -9376,10 +9376,10 @@
       <c r="B29" s="21"/>
       <c r="C29" s="22"/>
       <c r="D29" s="44" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F29" s="44" t="s">
         <v>63</v>
@@ -9401,10 +9401,10 @@
       <c r="B30" s="21"/>
       <c r="C30" s="22"/>
       <c r="D30" s="44" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F30" s="44" t="s">
         <v>63</v>
@@ -9426,10 +9426,10 @@
       <c r="B31" s="21"/>
       <c r="C31" s="22"/>
       <c r="D31" s="44" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F31" s="44" t="s">
         <v>63</v>
@@ -9451,10 +9451,10 @@
       <c r="B32" s="21"/>
       <c r="C32" s="22"/>
       <c r="D32" s="44" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F32" s="44" t="s">
         <v>63</v>
@@ -9471,15 +9471,15 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="44" t="s">
-        <v>782</v>
+        <v>793</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="22"/>
       <c r="D33" s="44" t="s">
-        <v>783</v>
+        <v>792</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F33" s="44" t="s">
         <v>63</v>
@@ -9496,11 +9496,11 @@
     </row>
     <row r="34" spans="1:9" s="22" customFormat="1">
       <c r="A34" s="44" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B34" s="21"/>
       <c r="D34" s="44" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="F34" s="44" t="s">
         <v>64</v>
@@ -9517,11 +9517,11 @@
     </row>
     <row r="35" spans="1:9" s="22" customFormat="1">
       <c r="A35" s="44" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B35" s="21"/>
       <c r="D35" s="44" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="F35" s="44" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Renamed measures class and name, updated test for 2x updated output variables
Also updated spreadsheets, but not results yet. I need to update post
processing scripts to handle new measure and variable names.
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="23460" tabRatio="562"/>
+    <workbookView xWindow="13420" yWindow="-20" windowWidth="37780" windowHeight="28260" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2166,24 +2166,12 @@
     <t>kBtu/ft^2</t>
   </si>
   <si>
-    <t>1.16.0</t>
-  </si>
-  <si>
     <t>../../measures</t>
   </si>
   <si>
     <t>../seeds/seed_empty.osm</t>
   </si>
   <si>
-    <t>BESTEST Building Thermal Envelope and Fabric Load Tests</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_tests</t>
-  </si>
-  <si>
-    <t>BESTESTBuildingThermalEnvelopeAndFabricLoadTests</t>
-  </si>
-  <si>
     <t>case_num</t>
   </si>
   <si>
@@ -2211,24 +2199,12 @@
     <t>../weather/USA_MA_Boston-Logan.Intl.AP.725090_TMY3.epw</t>
   </si>
   <si>
-    <t>BESTEST Building Thermal Envelope and Fabric Load Reports</t>
-  </si>
-  <si>
-    <t>BESTESTBuildingThermalEnvelopeAndFabricLoadReports</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports</t>
-  </si>
-  <si>
     <t>Annual Cooling</t>
   </si>
   <si>
     <t>MWh</t>
   </si>
   <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.annual_cooling</t>
-  </si>
-  <si>
     <t>Ann Clg (MWh)</t>
   </si>
   <si>
@@ -2238,9 +2214,6 @@
     <t>Ann Htg (MWh)</t>
   </si>
   <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.annual_heating</t>
-  </si>
-  <si>
     <t>Peak Heating Value</t>
   </si>
   <si>
@@ -2268,30 +2241,12 @@
     <t>Peak Cooling Time</t>
   </si>
   <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.peak_heating_value</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.peak_cooling_value</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.peak_cooling_time_display_name</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.peak_heating_time_display_name</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.sens_htg_clg_0104</t>
-  </si>
-  <si>
     <t>Annual Heating and Cooling</t>
   </si>
   <si>
     <t>Ann Htg and Clg</t>
   </si>
   <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.temp_0104</t>
-  </si>
-  <si>
     <t>Temperature January 4th</t>
   </si>
   <si>
@@ -2301,18 +2256,12 @@
     <t>C</t>
   </si>
   <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.temp_0727</t>
-  </si>
-  <si>
     <t>Temp 0727</t>
   </si>
   <si>
     <t>Temperature July 27th</t>
   </si>
   <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.surf_out_inst_slr_rad_0305_zone_surface_south</t>
-  </si>
-  <si>
     <t>Surface Incident South March 5th</t>
   </si>
   <si>
@@ -2331,9 +2280,6 @@
     <t>Temp Bins</t>
   </si>
   <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.temp_bins</t>
-  </si>
-  <si>
     <t>Min Temp</t>
   </si>
   <si>
@@ -2343,18 +2289,6 @@
     <t>Avg Temp</t>
   </si>
   <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.max_temp</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.min_temp</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.avg_temp</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.surf_out_inst_slr_rad_0305_zone_surface_west</t>
-  </si>
-  <si>
     <t>Surface Incident South July 27th</t>
   </si>
   <si>
@@ -2367,12 +2301,6 @@
     <t>Incident West 0727</t>
   </si>
   <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.surf_out_inst_slr_rad_0727_zone_surface_west</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.surf_out_inst_slr_rad_0727_zone_surface_south</t>
-  </si>
-  <si>
     <t>North Incident Solar</t>
   </si>
   <si>
@@ -2391,40 +2319,112 @@
     <t>kWh/m^2</t>
   </si>
   <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.north_incident_solar_radiation</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.east_incident_solar_radiation</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.west_incident_solar_radiation</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.horizontal_incident_solar_radiation</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.south_incident_solar_radiation</t>
-  </si>
-  <si>
     <t>Max Temp Position</t>
   </si>
   <si>
     <t>Min Temp Position</t>
   </si>
   <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.max_index_position</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.min_index_position</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports.zone_total_transmitted_solar_radiation</t>
-  </si>
-  <si>
     <t>Zone Total Transmitted Solar</t>
   </si>
   <si>
-    <t>BESTEST 1028_a (adjust door mat props to match wall)</t>
+    <t>1.17.0</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.annual_heating</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.annual_cooling</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.peak_heating_value</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.peak_cooling_value</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.peak_heating_time_display_name</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.peak_cooling_time_display_name</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.sens_htg_clg_0104</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.temp_0104</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.temp_0727</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.surf_out_inst_slr_rad_0305_zone_surface_south</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.surf_out_inst_slr_rad_0305_zone_surface_west</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.surf_out_inst_slr_rad_0727_zone_surface_south</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.surf_out_inst_slr_rad_0727_zone_surface_west</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.temp_bins</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.max_temp</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.min_temp</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.avg_temp</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.north_incident_solar_radiation</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.east_incident_solar_radiation</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.west_incident_solar_radiation</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.south_incident_solar_radiation</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.horizontal_incident_solar_radiation</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.zone_total_transmitted_solar_radiation</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.max_index_position</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.min_index_position</t>
+  </si>
+  <si>
+    <t>BESTEST Building Thermal Envelope and Fabric Load Reporting</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load_reporting</t>
+  </si>
+  <si>
+    <t>BESTESTBuildingThermalEnvelopeAndFabricLoadReporting</t>
+  </si>
+  <si>
+    <t>BESTEST Building Thermal Envelope and Fabric Load</t>
+  </si>
+  <si>
+    <t>bestest_building_thermal_envelope_and_fabric_load</t>
+  </si>
+  <si>
+    <t>BESTESTBuildingThermalEnvelopeAndFabricLoad</t>
+  </si>
+  <si>
+    <t>BESTEST Envelope 0512b</t>
   </si>
 </sst>
 </file>
@@ -2602,8 +2602,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1659">
+  <cellStyleXfs count="1661">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4359,7 +4361,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1659">
+  <cellStyles count="1661">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5189,6 +5191,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1654" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1656" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1660" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6018,6 +6021,7 @@
     <cellStyle name="Hyperlink" xfId="1653" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1655" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1659" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6380,7 +6384,7 @@
         <v>468</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>708</v>
+        <v>762</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>609</v>
@@ -6502,7 +6506,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -6822,7 +6826,7 @@
         <v>28</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" ht="28">
@@ -6854,7 +6858,7 @@
         <v>40</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>449</v>
@@ -6948,8 +6952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z53"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7133,13 +7137,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>711</v>
+        <v>791</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>712</v>
+        <v>792</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>713</v>
+        <v>793</v>
       </c>
       <c r="E4" s="36" t="s">
         <v>67</v>
@@ -7173,10 +7177,10 @@
       </c>
       <c r="C5" s="37"/>
       <c r="D5" s="37" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="F5" s="37"/>
       <c r="G5" s="37" t="s">
@@ -7184,26 +7188,26 @@
       </c>
       <c r="H5" s="37"/>
       <c r="I5" s="37" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="K5" s="37" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="L5" s="37" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="N5" s="37" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="43" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="Q5" s="41"/>
       <c r="R5" s="37" t="s">
@@ -7223,13 +7227,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>723</v>
+        <v>788</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>725</v>
+        <v>789</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>724</v>
+        <v>790</v>
       </c>
       <c r="E6" s="36" t="s">
         <v>232</v>
@@ -8593,7 +8597,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8781,14 +8785,14 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="15" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>707</v>
@@ -8928,16 +8932,16 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="44" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="D11" s="44" t="s">
-        <v>732</v>
+        <v>763</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>727</v>
+        <v>720</v>
       </c>
       <c r="F11" s="44" t="s">
         <v>63</v>
@@ -8949,22 +8953,22 @@
         <v>1</v>
       </c>
       <c r="I11" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="44" t="s">
-        <v>726</v>
+        <v>719</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
       <c r="C12" s="22"/>
       <c r="D12" s="44" t="s">
-        <v>728</v>
+        <v>764</v>
       </c>
       <c r="E12" s="44" t="s">
-        <v>727</v>
+        <v>720</v>
       </c>
       <c r="F12" s="44" t="s">
         <v>63</v>
@@ -8976,22 +8980,22 @@
         <v>1</v>
       </c>
       <c r="I12" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="44" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>738</v>
+        <v>729</v>
       </c>
       <c r="C13" s="22"/>
       <c r="D13" s="44" t="s">
-        <v>742</v>
+        <v>765</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>735</v>
+        <v>726</v>
       </c>
       <c r="F13" s="44" t="s">
         <v>63</v>
@@ -9003,22 +9007,22 @@
         <v>1</v>
       </c>
       <c r="I13" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="44" t="s">
-        <v>734</v>
+        <v>725</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>739</v>
+        <v>730</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="44" t="s">
-        <v>743</v>
+        <v>766</v>
       </c>
       <c r="E14" s="44" t="s">
-        <v>735</v>
+        <v>726</v>
       </c>
       <c r="F14" s="44" t="s">
         <v>63</v>
@@ -9030,18 +9034,18 @@
         <v>1</v>
       </c>
       <c r="I14" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="22" customFormat="1">
       <c r="A15" s="44" t="s">
-        <v>740</v>
+        <v>731</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>736</v>
+        <v>727</v>
       </c>
       <c r="D15" s="44" t="s">
-        <v>745</v>
+        <v>767</v>
       </c>
       <c r="E15" s="44"/>
       <c r="F15" s="44" t="s">
@@ -9054,18 +9058,18 @@
         <v>1</v>
       </c>
       <c r="I15" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="22" customFormat="1">
       <c r="A16" s="44" t="s">
-        <v>741</v>
+        <v>732</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>737</v>
+        <v>728</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>744</v>
+        <v>768</v>
       </c>
       <c r="E16" s="44"/>
       <c r="F16" s="44" t="s">
@@ -9078,18 +9082,18 @@
         <v>1</v>
       </c>
       <c r="I16" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="44" t="s">
-        <v>747</v>
+        <v>733</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="D17" s="44" t="s">
-        <v>746</v>
+        <v>769</v>
       </c>
       <c r="F17" s="44" t="s">
         <v>103</v>
@@ -9101,21 +9105,21 @@
         <v>1</v>
       </c>
       <c r="I17" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="44" t="s">
-        <v>750</v>
+        <v>735</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>751</v>
+        <v>736</v>
       </c>
       <c r="D18" s="44" t="s">
-        <v>749</v>
+        <v>770</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>752</v>
+        <v>737</v>
       </c>
       <c r="F18" s="44" t="s">
         <v>63</v>
@@ -9127,21 +9131,21 @@
         <v>1</v>
       </c>
       <c r="I18" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="44" t="s">
-        <v>755</v>
+        <v>739</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>754</v>
+        <v>738</v>
       </c>
       <c r="D19" s="44" t="s">
-        <v>753</v>
+        <v>771</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>752</v>
+        <v>737</v>
       </c>
       <c r="F19" s="44" t="s">
         <v>63</v>
@@ -9153,18 +9157,18 @@
         <v>1</v>
       </c>
       <c r="I19" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="44" t="s">
-        <v>757</v>
+        <v>740</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>759</v>
+        <v>742</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>756</v>
+        <v>772</v>
       </c>
       <c r="F20" s="44" t="s">
         <v>103</v>
@@ -9176,18 +9180,18 @@
         <v>1</v>
       </c>
       <c r="I20" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="44" t="s">
-        <v>758</v>
+        <v>741</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>760</v>
+        <v>743</v>
       </c>
       <c r="D21" s="44" t="s">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="F21" s="44" t="s">
         <v>103</v>
@@ -9199,18 +9203,18 @@
         <v>1</v>
       </c>
       <c r="I21" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="44" t="s">
-        <v>771</v>
+        <v>749</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>773</v>
+        <v>751</v>
       </c>
       <c r="D22" s="44" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="F22" s="44" t="s">
         <v>103</v>
@@ -9222,15 +9226,15 @@
         <v>1</v>
       </c>
       <c r="I22" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="44" t="s">
-        <v>772</v>
+        <v>750</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>774</v>
+        <v>752</v>
       </c>
       <c r="D23" s="44" t="s">
         <v>775</v>
@@ -9245,18 +9249,18 @@
         <v>1</v>
       </c>
       <c r="I23" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="44" t="s">
-        <v>761</v>
+        <v>744</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>762</v>
+        <v>745</v>
       </c>
       <c r="D24" s="44" t="s">
-        <v>763</v>
+        <v>776</v>
       </c>
       <c r="F24" s="44" t="s">
         <v>103</v>
@@ -9268,20 +9272,20 @@
         <v>1</v>
       </c>
       <c r="I24" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="44" t="s">
-        <v>765</v>
+        <v>747</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
       <c r="D25" s="44" t="s">
-        <v>767</v>
+        <v>777</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>752</v>
+        <v>737</v>
       </c>
       <c r="F25" s="44" t="s">
         <v>63</v>
@@ -9293,19 +9297,19 @@
         <v>1</v>
       </c>
       <c r="I25" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="44" t="s">
-        <v>764</v>
+        <v>746</v>
       </c>
       <c r="B26" s="21"/>
       <c r="D26" s="44" t="s">
-        <v>768</v>
+        <v>778</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>752</v>
+        <v>737</v>
       </c>
       <c r="F26" s="44" t="s">
         <v>63</v>
@@ -9317,19 +9321,19 @@
         <v>1</v>
       </c>
       <c r="I26" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="44" t="s">
-        <v>766</v>
+        <v>748</v>
       </c>
       <c r="B27" s="21"/>
       <c r="D27" s="44" t="s">
-        <v>769</v>
+        <v>779</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>752</v>
+        <v>737</v>
       </c>
       <c r="F27" s="44" t="s">
         <v>63</v>
@@ -9341,20 +9345,20 @@
         <v>1</v>
       </c>
       <c r="I27" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="44" t="s">
-        <v>777</v>
+        <v>753</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
       <c r="D28" s="44" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>782</v>
+        <v>758</v>
       </c>
       <c r="F28" s="44" t="s">
         <v>63</v>
@@ -9366,20 +9370,20 @@
         <v>1</v>
       </c>
       <c r="I28" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="44" t="s">
-        <v>778</v>
+        <v>754</v>
       </c>
       <c r="B29" s="21"/>
       <c r="C29" s="22"/>
       <c r="D29" s="44" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>782</v>
+        <v>758</v>
       </c>
       <c r="F29" s="44" t="s">
         <v>63</v>
@@ -9391,20 +9395,20 @@
         <v>1</v>
       </c>
       <c r="I29" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="44" t="s">
-        <v>779</v>
+        <v>755</v>
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="22"/>
       <c r="D30" s="44" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>782</v>
+        <v>758</v>
       </c>
       <c r="F30" s="44" t="s">
         <v>63</v>
@@ -9416,20 +9420,20 @@
         <v>1</v>
       </c>
       <c r="I30" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="44" t="s">
-        <v>780</v>
+        <v>756</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="22"/>
       <c r="D31" s="44" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>782</v>
+        <v>758</v>
       </c>
       <c r="F31" s="44" t="s">
         <v>63</v>
@@ -9441,20 +9445,20 @@
         <v>1</v>
       </c>
       <c r="I31" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="44" t="s">
-        <v>781</v>
+        <v>757</v>
       </c>
       <c r="B32" s="21"/>
       <c r="C32" s="22"/>
       <c r="D32" s="44" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>782</v>
+        <v>758</v>
       </c>
       <c r="F32" s="44" t="s">
         <v>63</v>
@@ -9466,20 +9470,20 @@
         <v>1</v>
       </c>
       <c r="I32" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="44" t="s">
-        <v>793</v>
+        <v>761</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="22"/>
       <c r="D33" s="44" t="s">
-        <v>792</v>
+        <v>785</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>782</v>
+        <v>758</v>
       </c>
       <c r="F33" s="44" t="s">
         <v>63</v>
@@ -9491,16 +9495,16 @@
         <v>1</v>
       </c>
       <c r="I33" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="22" customFormat="1">
       <c r="A34" s="44" t="s">
-        <v>788</v>
+        <v>759</v>
       </c>
       <c r="B34" s="21"/>
       <c r="D34" s="44" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="F34" s="44" t="s">
         <v>64</v>
@@ -9512,16 +9516,16 @@
         <v>1</v>
       </c>
       <c r="I34" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="22" customFormat="1">
       <c r="A35" s="44" t="s">
-        <v>789</v>
+        <v>760</v>
       </c>
       <c r="B35" s="21"/>
       <c r="D35" s="44" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="F35" s="44" t="s">
         <v>64</v>
@@ -9533,7 +9537,7 @@
         <v>1</v>
       </c>
       <c r="I35" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:9">

</xml_diff>

<commit_message>
Updated post processing and results for E+8.7 and OS 2.1.0
Only thing that jumped out was Figure B16.6-4.  Comparison of the Fan
Energy for the
Fuel-Fired Furnace Test Cases. Need to see why change in fans from 8.6
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_01.xlsx
+++ b/integration_testing/projects/bestest_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13420" yWindow="-20" windowWidth="37780" windowHeight="28260" tabRatio="562"/>
+    <workbookView xWindow="13420" yWindow="-20" windowWidth="37780" windowHeight="28260" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2343,12 +2343,6 @@
     <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.peak_cooling_value</t>
   </si>
   <si>
-    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.peak_heating_time_display_name</t>
-  </si>
-  <si>
-    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.peak_cooling_time_display_name</t>
-  </si>
-  <si>
     <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.sens_htg_clg_0104</t>
   </si>
   <si>
@@ -2425,6 +2419,12 @@
   </si>
   <si>
     <t>BESTEST Envelope 0512b</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.peak_heating_time</t>
+  </si>
+  <si>
+    <t>BestestBuildingThermalEnvelopeAndFabricLoadReporting.peak_cooling_time</t>
   </si>
 </sst>
 </file>
@@ -6323,7 +6323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -6495,7 +6495,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>470</v>
@@ -7137,13 +7137,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="36" t="s">
+        <v>789</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>790</v>
+      </c>
+      <c r="D4" s="36" t="s">
         <v>791</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>792</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>793</v>
       </c>
       <c r="E4" s="36" t="s">
         <v>67</v>
@@ -7227,13 +7227,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="36" t="s">
+        <v>786</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>787</v>
+      </c>
+      <c r="D6" s="36" t="s">
         <v>788</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>789</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>790</v>
       </c>
       <c r="E6" s="36" t="s">
         <v>232</v>
@@ -8595,9 +8595,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9045,7 +9045,7 @@
         <v>727</v>
       </c>
       <c r="D15" s="44" t="s">
-        <v>767</v>
+        <v>793</v>
       </c>
       <c r="E15" s="44"/>
       <c r="F15" s="44" t="s">
@@ -9069,7 +9069,7 @@
         <v>728</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>768</v>
+        <v>794</v>
       </c>
       <c r="E16" s="44"/>
       <c r="F16" s="44" t="s">
@@ -9093,7 +9093,7 @@
         <v>734</v>
       </c>
       <c r="D17" s="44" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="F17" s="44" t="s">
         <v>103</v>
@@ -9116,7 +9116,7 @@
         <v>736</v>
       </c>
       <c r="D18" s="44" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>737</v>
@@ -9142,7 +9142,7 @@
         <v>738</v>
       </c>
       <c r="D19" s="44" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="E19" s="22" t="s">
         <v>737</v>
@@ -9168,7 +9168,7 @@
         <v>742</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F20" s="44" t="s">
         <v>103</v>
@@ -9191,7 +9191,7 @@
         <v>743</v>
       </c>
       <c r="D21" s="44" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="F21" s="44" t="s">
         <v>103</v>
@@ -9214,7 +9214,7 @@
         <v>751</v>
       </c>
       <c r="D22" s="44" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="F22" s="44" t="s">
         <v>103</v>
@@ -9237,7 +9237,7 @@
         <v>752</v>
       </c>
       <c r="D23" s="44" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="F23" s="44" t="s">
         <v>103</v>
@@ -9260,7 +9260,7 @@
         <v>745</v>
       </c>
       <c r="D24" s="44" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="F24" s="44" t="s">
         <v>103</v>
@@ -9282,7 +9282,7 @@
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
       <c r="D25" s="44" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E25" s="22" t="s">
         <v>737</v>
@@ -9306,7 +9306,7 @@
       </c>
       <c r="B26" s="21"/>
       <c r="D26" s="44" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E26" s="22" t="s">
         <v>737</v>
@@ -9330,7 +9330,7 @@
       </c>
       <c r="B27" s="21"/>
       <c r="D27" s="44" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E27" s="22" t="s">
         <v>737</v>
@@ -9355,7 +9355,7 @@
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
       <c r="D28" s="44" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="E28" s="22" t="s">
         <v>758</v>
@@ -9380,7 +9380,7 @@
       <c r="B29" s="21"/>
       <c r="C29" s="22"/>
       <c r="D29" s="44" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E29" s="22" t="s">
         <v>758</v>
@@ -9405,7 +9405,7 @@
       <c r="B30" s="21"/>
       <c r="C30" s="22"/>
       <c r="D30" s="44" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="E30" s="22" t="s">
         <v>758</v>
@@ -9430,7 +9430,7 @@
       <c r="B31" s="21"/>
       <c r="C31" s="22"/>
       <c r="D31" s="44" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="E31" s="22" t="s">
         <v>758</v>
@@ -9455,7 +9455,7 @@
       <c r="B32" s="21"/>
       <c r="C32" s="22"/>
       <c r="D32" s="44" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="E32" s="22" t="s">
         <v>758</v>
@@ -9480,7 +9480,7 @@
       <c r="B33" s="21"/>
       <c r="C33" s="22"/>
       <c r="D33" s="44" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="E33" s="22" t="s">
         <v>758</v>
@@ -9504,7 +9504,7 @@
       </c>
       <c r="B34" s="21"/>
       <c r="D34" s="44" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="F34" s="44" t="s">
         <v>64</v>
@@ -9525,7 +9525,7 @@
       </c>
       <c r="B35" s="21"/>
       <c r="D35" s="44" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F35" s="44" t="s">
         <v>64</v>

</xml_diff>